<commit_message>
Created OfficeWorker and added rudimentary behavior. Added GameManager singleton and pausing methods. Modified GuardBehavior.cs to be more parallel to OfficeWorkerLogic.cs with regard to state switching; behavioral state changes will now be centralized in a single State property on each character. In theory this will make state changes easier to manage during interactions.
</commit_message>
<xml_diff>
--- a/JamTwo/Assets/Docs/SYNTW interactions.xlsx
+++ b/JamTwo/Assets/Docs/SYNTW interactions.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\JamTwoSaveSelf\JamTwo\Assets\Docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB82E61-BC97-4B10-A63C-1EF8F12FD799}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -310,93 +319,99 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="2">
-    <border/>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf quotePrefix="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -586,34 +601,39 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:AF26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A22:A26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="37.29"/>
-    <col customWidth="1" min="2" max="2" width="67.14"/>
-    <col customWidth="1" min="3" max="3" width="31.14"/>
-    <col customWidth="1" min="4" max="4" width="38.43"/>
-    <col customWidth="1" min="5" max="5" width="58.57"/>
-    <col customWidth="1" min="6" max="6" width="40.43"/>
-    <col customWidth="1" min="7" max="7" width="56.71"/>
-    <col customWidth="1" min="8" max="8" width="58.71"/>
-    <col customWidth="1" min="9" max="9" width="47.86"/>
-    <col customWidth="1" min="10" max="10" width="33.57"/>
-    <col customWidth="1" min="11" max="11" width="21.29"/>
-    <col customWidth="1" min="12" max="12" width="27.29"/>
+    <col min="1" max="1" width="37.28515625" customWidth="1"/>
+    <col min="2" max="2" width="67.140625" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" customWidth="1"/>
+    <col min="5" max="5" width="58.5703125" customWidth="1"/>
+    <col min="6" max="6" width="40.42578125" customWidth="1"/>
+    <col min="7" max="7" width="56.7109375" customWidth="1"/>
+    <col min="8" max="8" width="58.7109375" customWidth="1"/>
+    <col min="9" max="9" width="47.85546875" customWidth="1"/>
+    <col min="10" max="10" width="33.5703125" customWidth="1"/>
+    <col min="11" max="11" width="21.28515625" customWidth="1"/>
+    <col min="12" max="12" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -669,7 +689,7 @@
       <c r="AE1" s="3"/>
       <c r="AF1" s="3"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -704,7 +724,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
         <v>22</v>
       </c>
@@ -736,7 +756,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>31</v>
       </c>
@@ -778,7 +798,7 @@
       <c r="AE4" s="8"/>
       <c r="AF4" s="8"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>35</v>
       </c>
@@ -813,7 +833,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
         <v>45</v>
       </c>
@@ -845,7 +865,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>31</v>
       </c>
@@ -887,7 +907,7 @@
       <c r="AE7" s="8"/>
       <c r="AF7" s="8"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>56</v>
       </c>
@@ -922,7 +942,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
         <v>64</v>
       </c>
@@ -954,7 +974,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>31</v>
       </c>
@@ -996,7 +1016,7 @@
       <c r="AE10" s="8"/>
       <c r="AF10" s="8"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>75</v>
       </c>
@@ -1031,7 +1051,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
       <c r="B12" s="10" t="s">
         <v>85</v>
@@ -1085,38 +1105,38 @@
       <c r="AE12" s="8"/>
       <c r="AF12" s="8"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B21" s="1"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>97</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated interactions and added design.
</commit_message>
<xml_diff>
--- a/JamTwo/Assets/Docs/SYNTW interactions.xlsx
+++ b/JamTwo/Assets/Docs/SYNTW interactions.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Game_Jams\JamTwo\Assets\Docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="99">
   <si>
     <t>NPCs</t>
   </si>
@@ -305,98 +313,107 @@
   </si>
   <si>
     <t>Those clowns in Washington are at it again!</t>
+  </si>
+  <si>
+    <t>"We already talked today"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="2">
-    <border/>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf quotePrefix="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -586,34 +603,39 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:AF26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="37.29"/>
-    <col customWidth="1" min="2" max="2" width="67.14"/>
-    <col customWidth="1" min="3" max="3" width="31.14"/>
-    <col customWidth="1" min="4" max="4" width="38.43"/>
-    <col customWidth="1" min="5" max="5" width="58.57"/>
-    <col customWidth="1" min="6" max="6" width="40.43"/>
-    <col customWidth="1" min="7" max="7" width="56.71"/>
-    <col customWidth="1" min="8" max="8" width="58.71"/>
-    <col customWidth="1" min="9" max="9" width="47.86"/>
-    <col customWidth="1" min="10" max="10" width="33.57"/>
-    <col customWidth="1" min="11" max="11" width="21.29"/>
-    <col customWidth="1" min="12" max="12" width="27.29"/>
+    <col min="1" max="1" width="37.28515625" customWidth="1"/>
+    <col min="2" max="2" width="67.140625" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" customWidth="1"/>
+    <col min="5" max="5" width="58.5703125" customWidth="1"/>
+    <col min="6" max="6" width="40.42578125" customWidth="1"/>
+    <col min="7" max="7" width="56.7109375" customWidth="1"/>
+    <col min="8" max="8" width="58.7109375" customWidth="1"/>
+    <col min="9" max="9" width="47.85546875" customWidth="1"/>
+    <col min="10" max="10" width="33.5703125" customWidth="1"/>
+    <col min="11" max="11" width="21.28515625" customWidth="1"/>
+    <col min="12" max="12" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -669,7 +691,7 @@
       <c r="AE1" s="3"/>
       <c r="AF1" s="3"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -704,7 +726,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
         <v>22</v>
       </c>
@@ -736,7 +758,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>31</v>
       </c>
@@ -778,7 +800,7 @@
       <c r="AE4" s="8"/>
       <c r="AF4" s="8"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>35</v>
       </c>
@@ -813,7 +835,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
         <v>45</v>
       </c>
@@ -845,7 +867,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>31</v>
       </c>
@@ -887,7 +909,7 @@
       <c r="AE7" s="8"/>
       <c r="AF7" s="8"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>56</v>
       </c>
@@ -922,7 +944,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
         <v>64</v>
       </c>
@@ -954,7 +976,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>31</v>
       </c>
@@ -996,7 +1018,7 @@
       <c r="AE10" s="8"/>
       <c r="AF10" s="8"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>75</v>
       </c>
@@ -1031,7 +1053,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
       <c r="B12" s="10" t="s">
         <v>85</v>
@@ -1085,38 +1107,40 @@
       <c r="AE12" s="8"/>
       <c r="AF12" s="8"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="1"/>
-    </row>
-    <row r="22">
+      <c r="B21" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>97</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>